<commit_message>
More conversions to set up new table structure
</commit_message>
<xml_diff>
--- a/Decoupling/DecouplingLitDataNew.xlsx
+++ b/Decoupling/DecouplingLitDataNew.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{CB2CF81C-4C7E-4F2E-BCA7-7A602E7EE33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4096AE48-D47B-40B7-AAAF-156C1869352B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{CB2CF81C-4C7E-4F2E-BCA7-7A602E7EE33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0FBFDA72-9011-4BCD-BA31-5C7A0519E68D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
     <definedName name="yc">#REF!</definedName>
     <definedName name="ys">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3402,17 +3402,17 @@
   <dimension ref="A1:DS114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="21.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" style="1" customWidth="1"/>
     <col min="4" max="114" width="12.6328125" style="1" customWidth="1"/>
     <col min="115" max="16384" width="8.6328125" style="1"/>
   </cols>
@@ -17124,18 +17124,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17158,18 +17158,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADE82811-FB94-47CF-8920-BB36AEDBEBCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E37C02-1418-445A-A03B-8A00FF8D80E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADE82811-FB94-47CF-8920-BB36AEDBEBCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Inital add of all new cases for the calcLists function
</commit_message>
<xml_diff>
--- a/Decoupling/DecouplingLitDataNew.xlsx
+++ b/Decoupling/DecouplingLitDataNew.xlsx
@@ -3402,10 +3402,10 @@
   <dimension ref="A1:DS114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B81" sqref="B81"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15.5"/>
@@ -17124,18 +17124,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17158,18 +17158,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADE82811-FB94-47CF-8920-BB36AEDBEBCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E37C02-1418-445A-A03B-8A00FF8D80E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADE82811-FB94-47CF-8920-BB36AEDBEBCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>